<commit_message>
Chlor-a transformations look to be a little unreliable so wait to publish those until we have more data
</commit_message>
<xml_diff>
--- a/gl4.buoy.PMEC7.meta.xlsx
+++ b/gl4.buoy.PMEC7.meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GL4 Sensor/Buoy Data/Buoy_QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{216FB1E1-EC6D-134E-B340-54AFB49B11C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B840CD-D486-4B47-AF8F-F0336A784D8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,7 +677,7 @@
     <t xml:space="preserve"> Q is the ratio of the [DO] as determined from emission intensity to the [DO] as determined by emission lifetime.</t>
   </si>
   <si>
-    <t>gl4.buoy.PMEDO.data.csv</t>
+    <t>gl4.buoy.PMEC7.data.csv</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add in details about PAR acceleration meterics for X Y or Z. QA'QCed data to 2 SD to minimize amount of readings with a tilt.
</commit_message>
<xml_diff>
--- a/gl4.buoy.PMEC7.meta.xlsx
+++ b/gl4.buoy.PMEC7.meta.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GL4 Sensor/Buoy Data/Buoy_QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B840CD-D486-4B47-AF8F-F0336A784D8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA3620E-AD2F-7446-B56D-C4EAD735DA3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="920" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="gl4_bouy.PMEDO.meta" sheetId="2" r:id="rId2"/>
+    <sheet name="gl4_bouy.PMEC7.meta" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="disciplines">metadata!$T$2:$T$13</definedName>
@@ -599,9 +599,6 @@
     <t>measurement time in 30 minute intervals in mountain standard time</t>
   </si>
   <si>
-    <t>dissolved oxygen</t>
-  </si>
-  <si>
     <t>lake metabolism</t>
   </si>
   <si>
@@ -679,6 +676,9 @@
   <si>
     <t>gl4.buoy.PMEC7.data.csv</t>
   </si>
+  <si>
+    <t>chlorophyll-a</t>
+  </si>
 </sst>
 </file>
 
@@ -688,7 +688,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -735,6 +735,25 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -936,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -979,7 +998,6 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1001,6 +1019,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1372,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1392,14 +1415,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1483,10 +1506,10 @@
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="7"/>
@@ -1515,10 +1538,10 @@
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="7"/>
@@ -1547,10 +1570,10 @@
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="7"/>
@@ -1579,10 +1602,10 @@
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>122</v>
       </c>
       <c r="D7" s="7"/>
@@ -1611,10 +1634,10 @@
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="2"/>
@@ -1641,10 +1664,10 @@
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="7"/>
@@ -1673,10 +1696,10 @@
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="7"/>
@@ -1705,10 +1728,10 @@
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="34">
         <v>80309</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>80309</v>
       </c>
       <c r="D11" s="7"/>
@@ -1737,8 +1760,8 @@
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="2"/>
@@ -1765,10 +1788,10 @@
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>123</v>
       </c>
       <c r="D13" s="7"/>
@@ -1847,8 +1870,8 @@
       <c r="A16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="37" t="s">
-        <v>191</v>
+      <c r="B16" s="36" t="s">
+        <v>190</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1931,7 +1954,7 @@
       <c r="A19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>130</v>
       </c>
       <c r="C19" s="2"/>
@@ -2433,9 +2456,9 @@
       <c r="A37" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="31"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="19"/>
-      <c r="D37" s="31"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
@@ -2515,23 +2538,23 @@
       <c r="A40" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E40" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="F40" s="38" t="s">
+      <c r="F40" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G40" s="37" t="s">
         <v>165</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>166</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -3112,10 +3135,10 @@
       <c r="B63" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="31" t="s">
         <v>135</v>
       </c>
       <c r="E63" s="29"/>
@@ -3136,27 +3159,27 @@
       <c r="T63" s="2"/>
     </row>
     <row r="64" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="34">
+      <c r="A64" s="33">
         <v>2</v>
       </c>
-      <c r="B64" s="39" t="s">
+      <c r="B64" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="32" t="s">
+      <c r="D64" s="31" t="s">
         <v>159</v>
       </c>
       <c r="E64" s="29"/>
-      <c r="F64" s="42" t="s">
+      <c r="F64" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="G64" s="41" t="s">
         <v>56</v>
       </c>
       <c r="H64" s="29"/>
-      <c r="I64" s="32" t="s">
+      <c r="I64" s="31" t="s">
         <v>161</v>
       </c>
       <c r="J64" s="2"/>
@@ -3172,13 +3195,13 @@
       <c r="T64" s="2"/>
     </row>
     <row r="65" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="34">
+      <c r="A65" s="33">
         <v>3</v>
       </c>
-      <c r="B65" s="39" t="s">
+      <c r="B65" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="31" t="s">
         <v>137</v>
       </c>
       <c r="D65" s="29" t="s">
@@ -3208,27 +3231,27 @@
       <c r="T65" s="2"/>
     </row>
     <row r="66" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="34">
+      <c r="A66" s="33">
         <v>4</v>
       </c>
-      <c r="B66" s="39" t="s">
+      <c r="B66" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D66" s="32" t="s">
+      <c r="D66" s="31" t="s">
         <v>163</v>
       </c>
       <c r="E66" s="29"/>
-      <c r="F66" s="40">
+      <c r="F66" s="39">
         <v>43284.541666666664</v>
       </c>
-      <c r="G66" s="41">
+      <c r="G66" s="40">
         <v>43333</v>
       </c>
       <c r="H66" s="29"/>
-      <c r="I66" s="32" t="s">
+      <c r="I66" s="31" t="s">
         <v>164</v>
       </c>
       <c r="J66" s="2"/>
@@ -3244,29 +3267,29 @@
       <c r="T66" s="2"/>
     </row>
     <row r="67" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="34">
+      <c r="A67" s="33">
         <v>5</v>
       </c>
-      <c r="B67" s="39" t="s">
+      <c r="B67" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D67" s="32" t="s">
+      <c r="D67" s="31" t="s">
         <v>138</v>
       </c>
       <c r="E67" s="29"/>
-      <c r="F67" s="42">
+      <c r="F67" s="41">
         <v>0.4</v>
       </c>
-      <c r="G67" s="42">
+      <c r="G67" s="41">
         <v>11.5</v>
       </c>
       <c r="H67" s="29">
         <v>0.25</v>
       </c>
-      <c r="I67" s="32" t="s">
+      <c r="I67" s="31" t="s">
         <v>139</v>
       </c>
       <c r="J67" s="2"/>
@@ -3282,16 +3305,16 @@
       <c r="T67" s="2"/>
     </row>
     <row r="68" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="34">
+      <c r="A68" s="33">
         <v>6</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D68" s="32" t="s">
+      <c r="D68" s="31" t="s">
         <v>142</v>
       </c>
       <c r="E68" s="29"/>
@@ -3304,7 +3327,7 @@
       <c r="H68" s="29">
         <v>2E-3</v>
       </c>
-      <c r="I68" s="32" t="s">
+      <c r="I68" s="31" t="s">
         <v>141</v>
       </c>
       <c r="J68" s="2"/>
@@ -3320,17 +3343,17 @@
       <c r="T68" s="2"/>
     </row>
     <row r="69" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="34">
+      <c r="A69" s="33">
         <v>7</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>137</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E69" s="29"/>
       <c r="F69" s="29">
@@ -3343,7 +3366,7 @@
         <v>0.01</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3358,21 +3381,21 @@
       <c r="T69" s="2"/>
     </row>
     <row r="70" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="34">
+      <c r="A70" s="33">
         <v>8</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C70" s="29"/>
       <c r="D70" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E70" s="29"/>
-      <c r="F70" s="43">
+      <c r="F70" s="42">
         <v>44.5</v>
       </c>
-      <c r="G70" s="43">
+      <c r="G70" s="42">
         <v>111.25</v>
       </c>
       <c r="H70" s="29">
@@ -3392,17 +3415,17 @@
       <c r="T70" s="2"/>
     </row>
     <row r="71" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="34">
+      <c r="A71" s="33">
         <v>9</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
-      <c r="C71" s="32" t="s">
+      <c r="C71" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D71" s="32" t="s">
-        <v>185</v>
+      <c r="D71" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29">
@@ -3413,7 +3436,7 @@
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -3428,17 +3451,17 @@
       <c r="T71" s="2"/>
     </row>
     <row r="72" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="34">
+      <c r="A72" s="33">
         <v>10</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
-      <c r="C72" s="32" t="s">
+      <c r="C72" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="32" t="s">
-        <v>189</v>
+      <c r="D72" s="31" t="s">
+        <v>188</v>
       </c>
       <c r="E72" s="29"/>
       <c r="F72" s="29">
@@ -3449,7 +3472,7 @@
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -3464,7 +3487,7 @@
       <c r="T72" s="2"/>
     </row>
     <row r="73" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="34">
+      <c r="A73" s="33">
         <v>11</v>
       </c>
       <c r="B73" s="28"/>
@@ -3488,7 +3511,7 @@
       <c r="T73" s="2"/>
     </row>
     <row r="74" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="34">
+      <c r="A74" s="33">
         <v>12</v>
       </c>
       <c r="B74" s="28"/>
@@ -3512,7 +3535,7 @@
       <c r="T74" s="2"/>
     </row>
     <row r="75" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="34">
+      <c r="A75" s="33">
         <v>13</v>
       </c>
       <c r="B75" s="28"/>
@@ -3536,7 +3559,7 @@
       <c r="T75" s="2"/>
     </row>
     <row r="76" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="34">
+      <c r="A76" s="33">
         <v>14</v>
       </c>
       <c r="B76" s="28"/>
@@ -3560,7 +3583,7 @@
       <c r="T76" s="2"/>
     </row>
     <row r="77" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="34">
+      <c r="A77" s="33">
         <v>15</v>
       </c>
       <c r="B77" s="28"/>
@@ -3584,7 +3607,7 @@
       <c r="T77" s="2"/>
     </row>
     <row r="78" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="34">
+      <c r="A78" s="33">
         <v>16</v>
       </c>
       <c r="B78" s="28"/>
@@ -3608,7 +3631,7 @@
       <c r="T78" s="2"/>
     </row>
     <row r="79" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="34">
+      <c r="A79" s="33">
         <v>17</v>
       </c>
       <c r="B79" s="28"/>
@@ -3632,7 +3655,7 @@
       <c r="T79" s="2"/>
     </row>
     <row r="80" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="34">
+      <c r="A80" s="33">
         <v>18</v>
       </c>
       <c r="B80" s="28"/>
@@ -3656,7 +3679,7 @@
       <c r="T80" s="2"/>
     </row>
     <row r="81" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="34">
+      <c r="A81" s="33">
         <v>19</v>
       </c>
       <c r="B81" s="28"/>
@@ -23924,7 +23947,7 @@
   <dimension ref="A1:H989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24085,7 +24108,7 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="45" t="s">
         <v>147</v>
       </c>
       <c r="B14" s="2"/>
@@ -24097,8 +24120,8 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
-        <v>174</v>
+      <c r="A15" s="46" t="s">
+        <v>173</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -24109,8 +24132,8 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="33" t="s">
-        <v>175</v>
+      <c r="A16" s="47" t="s">
+        <v>174</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -24121,8 +24144,8 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
-        <v>176</v>
+      <c r="A17" s="46" t="s">
+        <v>175</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -24133,8 +24156,8 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>177</v>
+      <c r="A18" s="47" t="s">
+        <v>176</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -24144,14 +24167,16 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="33" t="s">
-        <v>178</v>
+    <row r="19" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="47" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="47"/>
+    </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -24161,7 +24186,7 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="45" t="s">
         <v>148</v>
       </c>
       <c r="B22" s="2"/>
@@ -24173,7 +24198,7 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="47" t="s">
         <v>149</v>
       </c>
       <c r="B23" s="2"/>
@@ -24185,7 +24210,7 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="47" t="s">
         <v>150</v>
       </c>
       <c r="B24" s="2"/>
@@ -24197,7 +24222,7 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="47" t="s">
         <v>152</v>
       </c>
       <c r="B25" s="2"/>
@@ -24209,7 +24234,7 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="47" t="s">
         <v>151</v>
       </c>
       <c r="B26" s="2"/>
@@ -24221,7 +24246,7 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="47" t="s">
         <v>153</v>
       </c>
       <c r="B27" s="2"/>
@@ -24232,13 +24257,13 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="33" t="s">
-        <v>179</v>
+    <row r="28" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="47" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="47" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="2"/>
@@ -24249,28 +24274,28 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="33" t="s">
-        <v>180</v>
+    <row r="30" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="47" t="s">
+        <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="47" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="33" t="s">
+    <row r="33" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="47" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="33" t="s">
-        <v>188</v>
-      </c>
-    </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="47" t="s">
         <v>155</v>
       </c>
       <c r="B34" s="2"/>
@@ -24282,8 +24307,8 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="33" t="s">
-        <v>181</v>
+      <c r="A35" s="47" t="s">
+        <v>180</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -24294,7 +24319,7 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -24304,7 +24329,7 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="45" t="s">
         <v>59</v>
       </c>
       <c r="B37" s="2"/>
@@ -24316,8 +24341,8 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="33" t="s">
-        <v>182</v>
+      <c r="A38" s="47" t="s">
+        <v>181</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -24327,13 +24352,13 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="33" t="s">
-        <v>183</v>
+    <row r="39" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="47" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="47" t="s">
         <v>156</v>
       </c>
       <c r="B40" s="2"/>
@@ -24365,7 +24390,7 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="33"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>

</xml_diff>